<commit_message>
Contextualización de los datos
</commit_message>
<xml_diff>
--- a/Trabajo_patrones_puntuales/Metadato.xlsx
+++ b/Trabajo_patrones_puntuales/Metadato.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\2022-1\Estadistica Espacial\Trabajo Procesos Puntuales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\GitHub\Patrones-puntuales\Trabajo_patrones_puntuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BB1FFBE-DEB4-467F-A396-2D40AB921492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6750"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Nombre de Columna</t>
   </si>
@@ -36,15 +35,9 @@
     <t>Tipo</t>
   </si>
   <si>
-    <t>Texto simple</t>
-  </si>
-  <si>
     <t>Número</t>
   </si>
   <si>
-    <t>objectid</t>
-  </si>
-  <si>
     <t>id_punto</t>
   </si>
   <si>
@@ -69,31 +62,37 @@
     <t>latitud</t>
   </si>
   <si>
-    <t>Nombre del establecimiento disponible para recarga de Civica</t>
-  </si>
-  <si>
-    <t>Dirección del establecimiento de recarga de Civica</t>
-  </si>
-  <si>
-    <t>Municipio del establecimiento de recarga de Civica</t>
-  </si>
-  <si>
-    <t>Barrio del establecimiento de recarga de Civica</t>
-  </si>
-  <si>
-    <t>Estado del establecimiento de recarga de Civica</t>
-  </si>
-  <si>
-    <t>Longuitud de las localizaciones de los establecimientos de recarga de Civica</t>
-  </si>
-  <si>
-    <t>Latitud de las localizaciones de los establecimientos de recarga de Civica</t>
+    <t>Nombre del establecimiento disponible para recarga de la tarjeta Cívica</t>
+  </si>
+  <si>
+    <t>Dirección del establecimiento de recarga de la tarjeta Cívica</t>
+  </si>
+  <si>
+    <t>Municipio del establecimiento de recarga de la tarjeta Cívica</t>
+  </si>
+  <si>
+    <t>Longuitud de las localizaciones de los establecimientos de recarga de la tarjeta Cívica</t>
+  </si>
+  <si>
+    <t>Latitud de las localizaciones de los establecimientos de recarga de la tarjeta Cívica</t>
+  </si>
+  <si>
+    <t>Identificador del punto de recarga de la tarjeta Cívica</t>
+  </si>
+  <si>
+    <t>Barrio del establecimiento de recarga de la tarjeta Cívica</t>
+  </si>
+  <si>
+    <t>Estado del establecimiento de recarga de la tarjeta Cívica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texto </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,21 +475,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.54296875" customWidth="1"/>
-    <col min="2" max="2" width="47.81640625" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -502,112 +501,104 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
+      <c r="C5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>4</v>
-      </c>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>